<commit_message>
fixed 4 scripts in icdc
</commit_message>
<xml_diff>
--- a/InputFiles/TC22_Canine_StudyUBC02-AllBreeds_StageOfDisease.xlsx
+++ b/InputFiles/TC22_Canine_StudyUBC02-AllBreeds_StageOfDisease.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4334A87E-2821-4CDE-A8E6-971BCEA58C17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FD6525-7D7E-4A9F-9399-AF44A837BAE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>